<commit_message>
Add riding_binplot function, riding_binplot vignette, and various other tweaks.
</commit_message>
<xml_diff>
--- a/data-raw/canada_squares.xlsx
+++ b/data-raw/canada_squares.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewmccormack/Desktop/mapcan/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewmccormack/Library/Containers/com.microsoft.Excel/Data/Desktop/mapcan/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B02A5B3-9739-2F47-A611-4A722B40C82A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895CE271-7D96-BA44-A602-43F64F35F32B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="480" windowWidth="25060" windowHeight="15540" activeTab="5" xr2:uid="{A76BE3CF-4497-F04C-A0EE-0244A10A98C8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="5" xr2:uid="{A76BE3CF-4497-F04C-A0EE-0244A10A98C8}"/>
   </bookViews>
   <sheets>
     <sheet name="representation_2013" sheetId="1" r:id="rId1"/>
     <sheet name="representation_2003" sheetId="3" r:id="rId2"/>
     <sheet name="representation_1996" sheetId="4" r:id="rId3"/>
-    <sheet name="representation_2013_breaks" sheetId="5" r:id="rId4"/>
-    <sheet name="representation_2003_breaks" sheetId="6" r:id="rId5"/>
-    <sheet name="representation_1996_breaks" sheetId="7" r:id="rId6"/>
+    <sheet name="representation_2003_breaks" sheetId="6" r:id="rId4"/>
+    <sheet name="representation_1996_breaks" sheetId="7" r:id="rId5"/>
+    <sheet name="representation_2013_breaks" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="13">
   <si>
     <t>BC</t>
   </si>
@@ -61,6 +61,15 @@
   <si>
     <t>NS</t>
   </si>
+  <si>
+    <t>NU</t>
+  </si>
+  <si>
+    <t>NT</t>
+  </si>
+  <si>
+    <t>YT</t>
+  </si>
 </sst>
 </file>
 
@@ -88,7 +97,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +146,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -150,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -166,6 +193,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5512,11 +5542,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307D6122-E4F2-E94C-9058-D00135335B95}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6599B2EE-3E3E-7E45-94DB-167FF5E33741}">
   <dimension ref="C1:BA40"/>
   <sheetViews>
     <sheetView zoomScale="43" workbookViewId="0">
-      <selection activeCell="AB14" sqref="AB14"/>
+      <selection activeCell="AL4" sqref="AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="36" customHeight="1"/>
@@ -5524,7 +5554,9 @@
     <col min="1" max="3" width="5.83203125" style="3"/>
     <col min="4" max="5" width="7" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="18" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" style="3" customWidth="1"/>
+    <col min="16" max="18" width="7" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="40" width="7.5" style="3" bestFit="1" customWidth="1"/>
     <col min="41" max="42" width="6.5" style="3" bestFit="1" customWidth="1"/>
     <col min="43" max="44" width="7.5" style="3" bestFit="1" customWidth="1"/>
@@ -5533,41 +5565,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:53" ht="36" customHeight="1">
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="T1" s="4"/>
       <c r="AJ1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AK1" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="AK1" s="4"/>
       <c r="AP1" s="4"/>
       <c r="AQ1" s="4"/>
       <c r="AR1" s="4"/>
       <c r="AS1" s="4"/>
     </row>
     <row r="2" spans="3:53" ht="36" customHeight="1">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="T2" s="4"/>
       <c r="AJ2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="AK2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM2" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
       <c r="AN2" s="4"/>
       <c r="AP2" s="4"/>
       <c r="AQ2" s="4"/>
@@ -5583,22 +5609,23 @@
     </row>
     <row r="3" spans="3:53" ht="36" customHeight="1">
       <c r="C3" s="1"/>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
       <c r="K3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="T3" s="4"/>
+      <c r="W3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="AJ3" s="5" t="s">
         <v>5</v>
       </c>
@@ -5641,12 +5668,8 @@
       <c r="I4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -5686,18 +5709,10 @@
       <c r="K5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
       <c r="Q5" s="5" t="s">
         <v>2</v>
       </c>
@@ -5789,24 +5804,12 @@
       <c r="U6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="W6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="X6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB6" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
       <c r="AE6" s="4"/>
@@ -5893,36 +5896,14 @@
       <c r="W7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="X7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG7" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
       <c r="AJ7" s="5" t="s">
         <v>5</v>
       </c>
@@ -6426,12 +6407,8 @@
       </c>
     </row>
     <row r="12" spans="3:53" ht="36" customHeight="1">
-      <c r="D12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
       <c r="W12" s="9" t="s">
         <v>4</v>
       </c>
@@ -6486,9 +6463,7 @@
       <c r="AP12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AQ12" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="AQ12" s="12"/>
       <c r="AR12" s="4"/>
       <c r="AU12" s="4"/>
       <c r="AV12" s="4"/>
@@ -6551,11 +6526,11 @@
       <c r="AM13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AN13" s="4"/>
       <c r="AO13" s="4"/>
       <c r="AP13" s="4"/>
       <c r="AQ13" s="4"/>
-      <c r="AS13" s="4"/>
+      <c r="AR13" s="4"/>
+      <c r="AU13" s="4"/>
       <c r="AY13" s="2" t="s">
         <v>9</v>
       </c>
@@ -6599,7 +6574,6 @@
       </c>
       <c r="AK14" s="4"/>
       <c r="AL14" s="4"/>
-      <c r="AM14" s="4"/>
     </row>
     <row r="15" spans="3:53" ht="36" customHeight="1">
       <c r="F15" s="11"/>
@@ -6643,6 +6617,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -6661,7 +6636,6 @@
       <c r="AD16" s="4"/>
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
-      <c r="AG16" s="4"/>
       <c r="AH16" s="9" t="s">
         <v>4</v>
       </c>
@@ -6680,11 +6654,11 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="4:46" ht="36" customHeight="1">
       <c r="D18" s="4"/>
@@ -6694,11 +6668,11 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="4:46" ht="36" customHeight="1">
       <c r="D19" s="4"/>
@@ -6708,11 +6682,11 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="4:46" ht="36" customHeight="1">
       <c r="D20" s="4"/>
@@ -6722,11 +6696,11 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="4:46" ht="36" customHeight="1">
       <c r="D21" s="4"/>
@@ -6736,11 +6710,11 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
     </row>
     <row r="22" spans="4:46" ht="36" customHeight="1">
       <c r="D22" s="4"/>
@@ -6770,6 +6744,25 @@
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="4"/>
+      <c r="AF25" s="4"/>
+      <c r="AG25" s="4"/>
+      <c r="AH25" s="4"/>
+      <c r="AI25" s="4"/>
       <c r="AJ25" s="4"/>
       <c r="AK25" s="4"/>
       <c r="AL25" s="4"/>
@@ -7211,11 +7204,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6599B2EE-3E3E-7E45-94DB-167FF5E33741}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4704963-84CE-D14F-93C7-AF27306E0631}">
   <dimension ref="C1:BA40"/>
   <sheetViews>
     <sheetView zoomScale="43" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+      <selection activeCell="AM13" sqref="AM13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="36" customHeight="1"/>
@@ -7223,9 +7216,7 @@
     <col min="1" max="3" width="5.83203125" style="3"/>
     <col min="4" max="5" width="7" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" style="3" customWidth="1"/>
-    <col min="16" max="18" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="18" width="7" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="40" width="7.5" style="3" bestFit="1" customWidth="1"/>
     <col min="41" max="42" width="6.5" style="3" bestFit="1" customWidth="1"/>
     <col min="43" max="44" width="7.5" style="3" bestFit="1" customWidth="1"/>
@@ -7247,7 +7238,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="J2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -7282,10 +7273,19 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="J3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="T3" s="4"/>
+      <c r="W3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="AJ3" s="5" t="s">
         <v>5</v>
       </c>
@@ -7322,13 +7322,9 @@
       <c r="G4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -7366,9 +7362,7 @@
       <c r="I5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -7396,7 +7390,7 @@
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
       <c r="AJ5" s="5" t="s">
         <v>5</v>
       </c>
@@ -7449,9 +7443,7 @@
       <c r="N6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="O6" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="O6" s="4"/>
       <c r="Q6" s="5" t="s">
         <v>2</v>
       </c>
@@ -7475,7 +7467,7 @@
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
-      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
       <c r="AJ6" s="5" t="s">
         <v>5</v>
       </c>
@@ -7668,10 +7660,8 @@
       <c r="AF8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AG8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH8" s="4"/>
+      <c r="AG8" s="4"/>
+      <c r="AI8" s="4"/>
       <c r="AJ8" s="5" t="s">
         <v>5</v>
       </c>
@@ -7785,9 +7775,7 @@
       <c r="AG9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AH9" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="AI9" s="4"/>
       <c r="AJ9" s="5" t="s">
         <v>5</v>
       </c>
@@ -7907,9 +7895,7 @@
       <c r="AG10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AH10" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="AI10" s="4"/>
       <c r="AM10" s="5" t="s">
         <v>5</v>
       </c>
@@ -8123,7 +8109,7 @@
       <c r="AP12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AQ12" s="12"/>
+      <c r="AQ12" s="4"/>
       <c r="AR12" s="4"/>
       <c r="AU12" s="4"/>
       <c r="AV12" s="4"/>
@@ -8277,7 +8263,6 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -8296,6 +8281,7 @@
       <c r="AD16" s="4"/>
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
+      <c r="AG16" s="4"/>
       <c r="AH16" s="9" t="s">
         <v>4</v>
       </c>
@@ -8306,7 +8292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="4:46" ht="36" customHeight="1">
+    <row r="17" spans="4:47" ht="36" customHeight="1">
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -8314,13 +8300,13 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="4:46" ht="36" customHeight="1">
+      <c r="Q17" s="4"/>
+    </row>
+    <row r="18" spans="4:47" ht="36" customHeight="1">
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -8328,13 +8314,13 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="4:46" ht="36" customHeight="1">
+      <c r="Q18" s="4"/>
+    </row>
+    <row r="19" spans="4:47" ht="36" customHeight="1">
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -8342,13 +8328,13 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="4:46" ht="36" customHeight="1">
+      <c r="Q19" s="4"/>
+    </row>
+    <row r="20" spans="4:47" ht="36" customHeight="1">
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -8356,13 +8342,13 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="4:46" ht="36" customHeight="1">
+      <c r="Q20" s="4"/>
+    </row>
+    <row r="21" spans="4:47" ht="36" customHeight="1">
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -8370,13 +8356,13 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="4:46" ht="36" customHeight="1">
+      <c r="Q21" s="4"/>
+    </row>
+    <row r="22" spans="4:47" ht="36" customHeight="1">
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -8384,26 +8370,27 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="4:46" ht="36" customHeight="1">
+      <c r="Q22" s="4"/>
+    </row>
+    <row r="23" spans="4:47" ht="36" customHeight="1">
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="4:46" ht="36" customHeight="1">
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="4:46" ht="36" customHeight="1">
-      <c r="L25" s="4"/>
+    <row r="24" spans="4:47" ht="36" customHeight="1">
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+    </row>
+    <row r="25" spans="4:47" ht="36" customHeight="1">
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
@@ -8423,6 +8410,1725 @@
       <c r="AG25" s="4"/>
       <c r="AH25" s="4"/>
       <c r="AI25" s="4"/>
+      <c r="AJ25" s="4"/>
+      <c r="AK25" s="4"/>
+      <c r="AL25" s="4"/>
+      <c r="AM25" s="4"/>
+      <c r="AN25" s="4"/>
+      <c r="AO25" s="4"/>
+      <c r="AP25" s="4"/>
+      <c r="AQ25" s="4"/>
+      <c r="AR25" s="4"/>
+      <c r="AS25" s="4"/>
+      <c r="AT25" s="4"/>
+      <c r="AU25" s="4"/>
+    </row>
+    <row r="26" spans="4:47" ht="36" customHeight="1">
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="4"/>
+      <c r="AF26" s="4"/>
+      <c r="AG26" s="4"/>
+      <c r="AH26" s="4"/>
+      <c r="AI26" s="4"/>
+      <c r="AJ26" s="4"/>
+      <c r="AK26" s="4"/>
+      <c r="AL26" s="4"/>
+      <c r="AM26" s="4"/>
+      <c r="AN26" s="4"/>
+      <c r="AO26" s="4"/>
+      <c r="AP26" s="4"/>
+      <c r="AQ26" s="4"/>
+      <c r="AR26" s="4"/>
+      <c r="AS26" s="4"/>
+      <c r="AT26" s="4"/>
+      <c r="AU26" s="4"/>
+    </row>
+    <row r="27" spans="4:47" ht="36" customHeight="1">
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="4"/>
+      <c r="AF27" s="4"/>
+      <c r="AG27" s="4"/>
+      <c r="AH27" s="4"/>
+      <c r="AI27" s="4"/>
+      <c r="AJ27" s="4"/>
+      <c r="AK27" s="4"/>
+      <c r="AL27" s="4"/>
+      <c r="AM27" s="4"/>
+      <c r="AN27" s="4"/>
+      <c r="AO27" s="4"/>
+      <c r="AP27" s="4"/>
+      <c r="AQ27" s="4"/>
+      <c r="AR27" s="4"/>
+    </row>
+    <row r="28" spans="4:47" ht="36" customHeight="1">
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
+      <c r="AE28" s="4"/>
+      <c r="AF28" s="4"/>
+      <c r="AG28" s="4"/>
+      <c r="AH28" s="4"/>
+      <c r="AI28" s="4"/>
+      <c r="AJ28" s="4"/>
+      <c r="AK28" s="4"/>
+      <c r="AL28" s="4"/>
+      <c r="AM28" s="4"/>
+    </row>
+    <row r="29" spans="4:47" ht="36" customHeight="1">
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4"/>
+      <c r="AI29" s="4"/>
+      <c r="AJ29" s="4"/>
+      <c r="AK29" s="4"/>
+      <c r="AL29" s="4"/>
+      <c r="AM29" s="4"/>
+    </row>
+    <row r="30" spans="4:47" ht="36" customHeight="1">
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4"/>
+      <c r="AE30" s="4"/>
+      <c r="AF30" s="4"/>
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="4"/>
+      <c r="AI30" s="4"/>
+      <c r="AJ30" s="4"/>
+      <c r="AK30" s="4"/>
+      <c r="AL30" s="4"/>
+      <c r="AM30" s="4"/>
+    </row>
+    <row r="31" spans="4:47" ht="36" customHeight="1">
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4"/>
+      <c r="AB31" s="4"/>
+      <c r="AC31" s="4"/>
+      <c r="AD31" s="4"/>
+      <c r="AE31" s="4"/>
+      <c r="AF31" s="4"/>
+      <c r="AG31" s="4"/>
+      <c r="AH31" s="4"/>
+      <c r="AI31" s="4"/>
+      <c r="AJ31" s="4"/>
+      <c r="AK31" s="4"/>
+      <c r="AL31" s="4"/>
+    </row>
+    <row r="32" spans="4:47" ht="36" customHeight="1">
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4"/>
+      <c r="AA32" s="4"/>
+      <c r="AB32" s="4"/>
+      <c r="AC32" s="4"/>
+      <c r="AD32" s="4"/>
+      <c r="AE32" s="4"/>
+      <c r="AF32" s="4"/>
+      <c r="AG32" s="4"/>
+      <c r="AH32" s="4"/>
+      <c r="AI32" s="4"/>
+      <c r="AJ32" s="4"/>
+      <c r="AK32" s="4"/>
+      <c r="AL32" s="4"/>
+    </row>
+    <row r="33" spans="12:38" ht="36" customHeight="1">
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="4"/>
+      <c r="AB33" s="4"/>
+      <c r="AC33" s="4"/>
+      <c r="AD33" s="4"/>
+      <c r="AE33" s="4"/>
+      <c r="AF33" s="4"/>
+      <c r="AG33" s="4"/>
+      <c r="AH33" s="4"/>
+      <c r="AI33" s="4"/>
+      <c r="AJ33" s="4"/>
+      <c r="AK33" s="4"/>
+      <c r="AL33" s="4"/>
+    </row>
+    <row r="34" spans="12:38" ht="36" customHeight="1">
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="4"/>
+      <c r="AB34" s="4"/>
+      <c r="AC34" s="4"/>
+      <c r="AD34" s="4"/>
+      <c r="AE34" s="4"/>
+      <c r="AF34" s="4"/>
+      <c r="AG34" s="4"/>
+      <c r="AH34" s="4"/>
+      <c r="AI34" s="4"/>
+      <c r="AJ34" s="4"/>
+      <c r="AK34" s="4"/>
+      <c r="AL34" s="4"/>
+    </row>
+    <row r="35" spans="12:38" ht="36" customHeight="1">
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4"/>
+      <c r="AA35" s="4"/>
+      <c r="AB35" s="4"/>
+      <c r="AC35" s="4"/>
+      <c r="AD35" s="4"/>
+      <c r="AE35" s="4"/>
+      <c r="AF35" s="4"/>
+      <c r="AG35" s="4"/>
+      <c r="AH35" s="4"/>
+      <c r="AI35" s="4"/>
+      <c r="AJ35" s="4"/>
+      <c r="AK35" s="4"/>
+      <c r="AL35" s="4"/>
+    </row>
+    <row r="36" spans="12:38" ht="36" customHeight="1">
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
+      <c r="AA36" s="4"/>
+      <c r="AB36" s="4"/>
+      <c r="AC36" s="4"/>
+      <c r="AD36" s="4"/>
+      <c r="AE36" s="4"/>
+      <c r="AF36" s="4"/>
+      <c r="AG36" s="4"/>
+      <c r="AH36" s="4"/>
+      <c r="AI36" s="4"/>
+      <c r="AJ36" s="4"/>
+      <c r="AK36" s="4"/>
+      <c r="AL36" s="4"/>
+    </row>
+    <row r="37" spans="12:38" ht="36" customHeight="1">
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4"/>
+      <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
+      <c r="AC37" s="4"/>
+      <c r="AD37" s="4"/>
+      <c r="AE37" s="4"/>
+      <c r="AF37" s="4"/>
+      <c r="AG37" s="4"/>
+      <c r="AH37" s="4"/>
+      <c r="AI37" s="4"/>
+      <c r="AJ37" s="4"/>
+      <c r="AK37" s="4"/>
+      <c r="AL37" s="4"/>
+    </row>
+    <row r="38" spans="12:38" ht="36" customHeight="1">
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
+      <c r="Z38" s="4"/>
+      <c r="AA38" s="4"/>
+      <c r="AB38" s="4"/>
+      <c r="AC38" s="4"/>
+      <c r="AD38" s="4"/>
+      <c r="AE38" s="4"/>
+      <c r="AF38" s="4"/>
+      <c r="AG38" s="4"/>
+      <c r="AH38" s="4"/>
+      <c r="AI38" s="4"/>
+      <c r="AJ38" s="4"/>
+      <c r="AK38" s="4"/>
+      <c r="AL38" s="4"/>
+    </row>
+    <row r="39" spans="12:38" ht="36" customHeight="1">
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="4"/>
+      <c r="AA39" s="4"/>
+      <c r="AB39" s="4"/>
+      <c r="AC39" s="4"/>
+      <c r="AD39" s="4"/>
+      <c r="AE39" s="4"/>
+      <c r="AF39" s="4"/>
+      <c r="AG39" s="4"/>
+      <c r="AH39" s="4"/>
+      <c r="AI39" s="4"/>
+      <c r="AJ39" s="4"/>
+      <c r="AK39" s="4"/>
+      <c r="AL39" s="4"/>
+    </row>
+    <row r="40" spans="12:38" ht="36" customHeight="1">
+      <c r="AD40" s="4"/>
+      <c r="AE40" s="4"/>
+      <c r="AF40" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307D6122-E4F2-E94C-9058-D00135335B95}">
+  <dimension ref="C1:BA40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="58" zoomScaleNormal="43" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="36" customHeight="1"/>
+  <cols>
+    <col min="1" max="3" width="5.83203125" style="3"/>
+    <col min="4" max="5" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="18" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="36" width="7.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.83203125" style="3" customWidth="1"/>
+    <col min="38" max="40" width="7.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="6.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="7.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="6.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="48" max="16384" width="5.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:53" ht="36" customHeight="1">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="AJ1" s="4"/>
+      <c r="AK1" s="4"/>
+      <c r="AP1" s="4"/>
+      <c r="AQ1" s="4"/>
+      <c r="AR1" s="4"/>
+      <c r="AS1" s="4"/>
+    </row>
+    <row r="2" spans="3:53" ht="36" customHeight="1">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="AJ2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4"/>
+    </row>
+    <row r="3" spans="3:53" ht="36" customHeight="1">
+      <c r="AJ3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN3" s="4"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AS3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AT3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="3:53" ht="36" customHeight="1">
+      <c r="C4" s="1"/>
+      <c r="F4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="W4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AS4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AT4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:53" ht="36" customHeight="1">
+      <c r="F5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="AJ5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="3:53" ht="36" customHeight="1">
+      <c r="C6" s="1"/>
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="4"/>
+      <c r="AJ6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AW6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AX6" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="3:53" ht="36" customHeight="1">
+      <c r="F7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="W7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="4"/>
+      <c r="AJ7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AW7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AX7" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="3:53" ht="36" customHeight="1">
+      <c r="F8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="BA8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="3:53" ht="36" customHeight="1">
+      <c r="F9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="W9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH9" s="4"/>
+      <c r="AJ9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="3:53" ht="36" customHeight="1">
+      <c r="F10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="W10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="3:53" ht="36" customHeight="1">
+      <c r="D11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="W11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AW11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="3:53" ht="36" customHeight="1">
+      <c r="D12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="W12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AW12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="3:53" ht="36" customHeight="1">
+      <c r="D13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR13" s="4"/>
+      <c r="AU13" s="4"/>
+      <c r="AV13" s="4"/>
+      <c r="AY13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ13" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="3:53" ht="36" customHeight="1">
+      <c r="W14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="X14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM14" s="4"/>
+      <c r="AN14" s="4"/>
+      <c r="AO14" s="4"/>
+      <c r="AP14" s="4"/>
+      <c r="AQ14" s="4"/>
+      <c r="AS14" s="4"/>
+      <c r="AY14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="3:53" ht="36" customHeight="1">
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK15" s="4"/>
+      <c r="AL15" s="4"/>
+      <c r="AM15" s="4"/>
+    </row>
+    <row r="16" spans="3:53" ht="36" customHeight="1">
+      <c r="F16" s="11"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK16" s="4"/>
+    </row>
+    <row r="17" spans="4:46" ht="36" customHeight="1">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ17" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="4:46" ht="36" customHeight="1">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="Q18" s="4"/>
+    </row>
+    <row r="19" spans="4:46" ht="36" customHeight="1">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="Q19" s="4"/>
+    </row>
+    <row r="20" spans="4:46" ht="36" customHeight="1">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="Q20" s="4"/>
+    </row>
+    <row r="21" spans="4:46" ht="36" customHeight="1">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+    </row>
+    <row r="22" spans="4:46" ht="36" customHeight="1">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="4:46" ht="36" customHeight="1">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="4:46" ht="36" customHeight="1">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="4:46" ht="36" customHeight="1">
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
       <c r="AJ25" s="4"/>
       <c r="AK25" s="4"/>
       <c r="AL25" s="4"/>
@@ -8861,1644 +10567,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4704963-84CE-D14F-93C7-AF27306E0631}">
-  <dimension ref="C1:BA40"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="43" workbookViewId="0">
-      <selection activeCell="BA28" sqref="BA28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="36" customHeight="1"/>
-  <cols>
-    <col min="1" max="3" width="5.83203125" style="3"/>
-    <col min="4" max="5" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="18" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="40" width="7.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="7.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="48" max="16384" width="5.83203125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="3:53" ht="36" customHeight="1">
-      <c r="AJ1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK1" s="4"/>
-      <c r="AP1" s="4"/>
-      <c r="AQ1" s="4"/>
-      <c r="AR1" s="4"/>
-      <c r="AS1" s="4"/>
-    </row>
-    <row r="2" spans="3:53" ht="36" customHeight="1">
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="AJ2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="4"/>
-      <c r="AP2" s="4"/>
-      <c r="AQ2" s="4"/>
-      <c r="AR2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AS2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AT2" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="3:53" ht="36" customHeight="1">
-      <c r="C3" s="1"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="AJ3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AQ3" s="4"/>
-      <c r="AR3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AS3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AT3" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="3:53" ht="36" customHeight="1">
-      <c r="F4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="AJ4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN4" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="3:53" ht="36" customHeight="1">
-      <c r="C5" s="1"/>
-      <c r="F5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="Q5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="4"/>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP5" s="4"/>
-      <c r="AQ5" s="4"/>
-      <c r="AW5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="AX5" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="3:53" ht="36" customHeight="1">
-      <c r="F6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O6" s="4"/>
-      <c r="Q6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="T6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="U6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
-      <c r="AF6" s="4"/>
-      <c r="AG6" s="4"/>
-      <c r="AI6" s="4"/>
-      <c r="AJ6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AW6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="AX6" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="3:53" ht="36" customHeight="1">
-      <c r="F7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="U7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="W7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="4"/>
-      <c r="AB7" s="4"/>
-      <c r="AC7" s="4"/>
-      <c r="AD7" s="4"/>
-      <c r="AE7" s="4"/>
-      <c r="AJ7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="BA7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="3:53" ht="36" customHeight="1">
-      <c r="F8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="R8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="T8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="U8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="W8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="X8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG8" s="4"/>
-      <c r="AI8" s="4"/>
-      <c r="AJ8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AU8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AV8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="BA8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="3:53" ht="36" customHeight="1">
-      <c r="F9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="T9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="U9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="W9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="X9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI9" s="4"/>
-      <c r="AJ9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AU9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AV9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="3:53" ht="36" customHeight="1">
-      <c r="D10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="T10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="U10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="W10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="X10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI10" s="4"/>
-      <c r="AM10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AU10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AV10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AW10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="3:53" ht="36" customHeight="1">
-      <c r="D11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="T11" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="U11" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="W11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="X11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AN11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AU11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AV11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AW11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="3:53" ht="36" customHeight="1">
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="W12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="X12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AL12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AO12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ12" s="4"/>
-      <c r="AR12" s="4"/>
-      <c r="AU12" s="4"/>
-      <c r="AV12" s="4"/>
-      <c r="AY12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="3:53" ht="36" customHeight="1">
-      <c r="W13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="X13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AL13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AM13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AO13" s="4"/>
-      <c r="AP13" s="4"/>
-      <c r="AQ13" s="4"/>
-      <c r="AR13" s="4"/>
-      <c r="AU13" s="4"/>
-      <c r="AY13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="3:53" ht="36" customHeight="1">
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK14" s="4"/>
-      <c r="AL14" s="4"/>
-    </row>
-    <row r="15" spans="3:53" ht="36" customHeight="1">
-      <c r="F15" s="11"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK15" s="4"/>
-    </row>
-    <row r="16" spans="3:53" ht="36" customHeight="1">
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
-      <c r="AB16" s="4"/>
-      <c r="AC16" s="4"/>
-      <c r="AD16" s="4"/>
-      <c r="AE16" s="4"/>
-      <c r="AF16" s="4"/>
-      <c r="AG16" s="4"/>
-      <c r="AH16" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI16" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ16" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="4:47" ht="36" customHeight="1">
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="Q17" s="4"/>
-    </row>
-    <row r="18" spans="4:47" ht="36" customHeight="1">
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="4:47" ht="36" customHeight="1">
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="Q19" s="4"/>
-    </row>
-    <row r="20" spans="4:47" ht="36" customHeight="1">
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="Q20" s="4"/>
-    </row>
-    <row r="21" spans="4:47" ht="36" customHeight="1">
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="Q21" s="4"/>
-    </row>
-    <row r="22" spans="4:47" ht="36" customHeight="1">
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="Q22" s="4"/>
-    </row>
-    <row r="23" spans="4:47" ht="36" customHeight="1">
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="4:47" ht="36" customHeight="1">
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-    </row>
-    <row r="25" spans="4:47" ht="36" customHeight="1">
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AA25" s="4"/>
-      <c r="AB25" s="4"/>
-      <c r="AC25" s="4"/>
-      <c r="AD25" s="4"/>
-      <c r="AE25" s="4"/>
-      <c r="AF25" s="4"/>
-      <c r="AG25" s="4"/>
-      <c r="AH25" s="4"/>
-      <c r="AI25" s="4"/>
-      <c r="AJ25" s="4"/>
-      <c r="AK25" s="4"/>
-      <c r="AL25" s="4"/>
-      <c r="AM25" s="4"/>
-      <c r="AN25" s="4"/>
-      <c r="AO25" s="4"/>
-      <c r="AP25" s="4"/>
-      <c r="AQ25" s="4"/>
-      <c r="AR25" s="4"/>
-      <c r="AS25" s="4"/>
-      <c r="AT25" s="4"/>
-      <c r="AU25" s="4"/>
-    </row>
-    <row r="26" spans="4:47" ht="36" customHeight="1">
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
-      <c r="AA26" s="4"/>
-      <c r="AB26" s="4"/>
-      <c r="AC26" s="4"/>
-      <c r="AD26" s="4"/>
-      <c r="AE26" s="4"/>
-      <c r="AF26" s="4"/>
-      <c r="AG26" s="4"/>
-      <c r="AH26" s="4"/>
-      <c r="AI26" s="4"/>
-      <c r="AJ26" s="4"/>
-      <c r="AK26" s="4"/>
-      <c r="AL26" s="4"/>
-      <c r="AM26" s="4"/>
-      <c r="AN26" s="4"/>
-      <c r="AO26" s="4"/>
-      <c r="AP26" s="4"/>
-      <c r="AQ26" s="4"/>
-      <c r="AR26" s="4"/>
-      <c r="AS26" s="4"/>
-      <c r="AT26" s="4"/>
-      <c r="AU26" s="4"/>
-    </row>
-    <row r="27" spans="4:47" ht="36" customHeight="1">
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-      <c r="AA27" s="4"/>
-      <c r="AB27" s="4"/>
-      <c r="AC27" s="4"/>
-      <c r="AD27" s="4"/>
-      <c r="AE27" s="4"/>
-      <c r="AF27" s="4"/>
-      <c r="AG27" s="4"/>
-      <c r="AH27" s="4"/>
-      <c r="AI27" s="4"/>
-      <c r="AJ27" s="4"/>
-      <c r="AK27" s="4"/>
-      <c r="AL27" s="4"/>
-      <c r="AM27" s="4"/>
-      <c r="AN27" s="4"/>
-      <c r="AO27" s="4"/>
-      <c r="AP27" s="4"/>
-      <c r="AQ27" s="4"/>
-      <c r="AR27" s="4"/>
-    </row>
-    <row r="28" spans="4:47" ht="36" customHeight="1">
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
-      <c r="AA28" s="4"/>
-      <c r="AB28" s="4"/>
-      <c r="AC28" s="4"/>
-      <c r="AD28" s="4"/>
-      <c r="AE28" s="4"/>
-      <c r="AF28" s="4"/>
-      <c r="AG28" s="4"/>
-      <c r="AH28" s="4"/>
-      <c r="AI28" s="4"/>
-      <c r="AJ28" s="4"/>
-      <c r="AK28" s="4"/>
-      <c r="AL28" s="4"/>
-      <c r="AM28" s="4"/>
-    </row>
-    <row r="29" spans="4:47" ht="36" customHeight="1">
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
-      <c r="AA29" s="4"/>
-      <c r="AB29" s="4"/>
-      <c r="AC29" s="4"/>
-      <c r="AD29" s="4"/>
-      <c r="AE29" s="4"/>
-      <c r="AF29" s="4"/>
-      <c r="AG29" s="4"/>
-      <c r="AH29" s="4"/>
-      <c r="AI29" s="4"/>
-      <c r="AJ29" s="4"/>
-      <c r="AK29" s="4"/>
-      <c r="AL29" s="4"/>
-      <c r="AM29" s="4"/>
-    </row>
-    <row r="30" spans="4:47" ht="36" customHeight="1">
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
-      <c r="Z30" s="4"/>
-      <c r="AA30" s="4"/>
-      <c r="AB30" s="4"/>
-      <c r="AC30" s="4"/>
-      <c r="AD30" s="4"/>
-      <c r="AE30" s="4"/>
-      <c r="AF30" s="4"/>
-      <c r="AG30" s="4"/>
-      <c r="AH30" s="4"/>
-      <c r="AI30" s="4"/>
-      <c r="AJ30" s="4"/>
-      <c r="AK30" s="4"/>
-      <c r="AL30" s="4"/>
-      <c r="AM30" s="4"/>
-    </row>
-    <row r="31" spans="4:47" ht="36" customHeight="1">
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-      <c r="Z31" s="4"/>
-      <c r="AA31" s="4"/>
-      <c r="AB31" s="4"/>
-      <c r="AC31" s="4"/>
-      <c r="AD31" s="4"/>
-      <c r="AE31" s="4"/>
-      <c r="AF31" s="4"/>
-      <c r="AG31" s="4"/>
-      <c r="AH31" s="4"/>
-      <c r="AI31" s="4"/>
-      <c r="AJ31" s="4"/>
-      <c r="AK31" s="4"/>
-      <c r="AL31" s="4"/>
-    </row>
-    <row r="32" spans="4:47" ht="36" customHeight="1">
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
-      <c r="AA32" s="4"/>
-      <c r="AB32" s="4"/>
-      <c r="AC32" s="4"/>
-      <c r="AD32" s="4"/>
-      <c r="AE32" s="4"/>
-      <c r="AF32" s="4"/>
-      <c r="AG32" s="4"/>
-      <c r="AH32" s="4"/>
-      <c r="AI32" s="4"/>
-      <c r="AJ32" s="4"/>
-      <c r="AK32" s="4"/>
-      <c r="AL32" s="4"/>
-    </row>
-    <row r="33" spans="12:38" ht="36" customHeight="1">
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
-      <c r="AA33" s="4"/>
-      <c r="AB33" s="4"/>
-      <c r="AC33" s="4"/>
-      <c r="AD33" s="4"/>
-      <c r="AE33" s="4"/>
-      <c r="AF33" s="4"/>
-      <c r="AG33" s="4"/>
-      <c r="AH33" s="4"/>
-      <c r="AI33" s="4"/>
-      <c r="AJ33" s="4"/>
-      <c r="AK33" s="4"/>
-      <c r="AL33" s="4"/>
-    </row>
-    <row r="34" spans="12:38" ht="36" customHeight="1">
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="4"/>
-      <c r="AA34" s="4"/>
-      <c r="AB34" s="4"/>
-      <c r="AC34" s="4"/>
-      <c r="AD34" s="4"/>
-      <c r="AE34" s="4"/>
-      <c r="AF34" s="4"/>
-      <c r="AG34" s="4"/>
-      <c r="AH34" s="4"/>
-      <c r="AI34" s="4"/>
-      <c r="AJ34" s="4"/>
-      <c r="AK34" s="4"/>
-      <c r="AL34" s="4"/>
-    </row>
-    <row r="35" spans="12:38" ht="36" customHeight="1">
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
-      <c r="AA35" s="4"/>
-      <c r="AB35" s="4"/>
-      <c r="AC35" s="4"/>
-      <c r="AD35" s="4"/>
-      <c r="AE35" s="4"/>
-      <c r="AF35" s="4"/>
-      <c r="AG35" s="4"/>
-      <c r="AH35" s="4"/>
-      <c r="AI35" s="4"/>
-      <c r="AJ35" s="4"/>
-      <c r="AK35" s="4"/>
-      <c r="AL35" s="4"/>
-    </row>
-    <row r="36" spans="12:38" ht="36" customHeight="1">
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="4"/>
-      <c r="AA36" s="4"/>
-      <c r="AB36" s="4"/>
-      <c r="AC36" s="4"/>
-      <c r="AD36" s="4"/>
-      <c r="AE36" s="4"/>
-      <c r="AF36" s="4"/>
-      <c r="AG36" s="4"/>
-      <c r="AH36" s="4"/>
-      <c r="AI36" s="4"/>
-      <c r="AJ36" s="4"/>
-      <c r="AK36" s="4"/>
-      <c r="AL36" s="4"/>
-    </row>
-    <row r="37" spans="12:38" ht="36" customHeight="1">
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
-      <c r="AA37" s="4"/>
-      <c r="AB37" s="4"/>
-      <c r="AC37" s="4"/>
-      <c r="AD37" s="4"/>
-      <c r="AE37" s="4"/>
-      <c r="AF37" s="4"/>
-      <c r="AG37" s="4"/>
-      <c r="AH37" s="4"/>
-      <c r="AI37" s="4"/>
-      <c r="AJ37" s="4"/>
-      <c r="AK37" s="4"/>
-      <c r="AL37" s="4"/>
-    </row>
-    <row r="38" spans="12:38" ht="36" customHeight="1">
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-      <c r="T38" s="4"/>
-      <c r="U38" s="4"/>
-      <c r="V38" s="4"/>
-      <c r="W38" s="4"/>
-      <c r="X38" s="4"/>
-      <c r="Y38" s="4"/>
-      <c r="Z38" s="4"/>
-      <c r="AA38" s="4"/>
-      <c r="AB38" s="4"/>
-      <c r="AC38" s="4"/>
-      <c r="AD38" s="4"/>
-      <c r="AE38" s="4"/>
-      <c r="AF38" s="4"/>
-      <c r="AG38" s="4"/>
-      <c r="AH38" s="4"/>
-      <c r="AI38" s="4"/>
-      <c r="AJ38" s="4"/>
-      <c r="AK38" s="4"/>
-      <c r="AL38" s="4"/>
-    </row>
-    <row r="39" spans="12:38" ht="36" customHeight="1">
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
-      <c r="W39" s="4"/>
-      <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-      <c r="Z39" s="4"/>
-      <c r="AA39" s="4"/>
-      <c r="AB39" s="4"/>
-      <c r="AC39" s="4"/>
-      <c r="AD39" s="4"/>
-      <c r="AE39" s="4"/>
-      <c r="AF39" s="4"/>
-      <c r="AG39" s="4"/>
-      <c r="AH39" s="4"/>
-      <c r="AI39" s="4"/>
-      <c r="AJ39" s="4"/>
-      <c r="AK39" s="4"/>
-      <c r="AL39" s="4"/>
-    </row>
-    <row r="40" spans="12:38" ht="36" customHeight="1">
-      <c r="AD40" s="4"/>
-      <c r="AE40" s="4"/>
-      <c r="AF40" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>